<commit_message>
new card stack (balanced) - 104 cards total
</commit_message>
<xml_diff>
--- a/data/Space_Goats_V1_Card_Deck2.xlsx
+++ b/data/Space_Goats_V1_Card_Deck2.xlsx
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -788,7 +788,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -821,7 +821,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -953,7 +953,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1019,7 +1019,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1216,7 +1216,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -1315,7 +1315,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1446,7 +1446,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1578,7 +1578,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -1611,7 +1611,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -1644,7 +1644,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change card allotment, market display 3 -> 4, unavoidable_ship_wreakage now is a "hit" instead of "destory"
</commit_message>
<xml_diff>
--- a/data/Space_Goats_V1_Card_Deck2.xlsx
+++ b/data/Space_Goats_V1_Card_Deck2.xlsx
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -821,7 +821,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -953,7 +953,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
major changes to card effects
</commit_message>
<xml_diff>
--- a/data/Space_Goats_V1_Card_Deck2.xlsx
+++ b/data/Space_Goats_V1_Card_Deck2.xlsx
@@ -911,12 +911,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>destroy_up_to_2_ships</t>
+          <t>destroy_up_to_2_ships_then_lose_one_1_bank_currency</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Two hits in one action</t>
+          <t>Two hits, then lose 1 bank currency</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>destroy_up_to_2_ships</t>
+          <t>destory_up_to_2_ships</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1141,12 +1141,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>assign_to_ship_block_1</t>
+          <t>assign_to_ship_block_1_draw_1_discard_1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Light defensive layer</t>
+          <t>Assign: block 1; immediately draw 1 then discard 1</t>
         </is>
       </c>
       <c r="G3" t="n">

</xml_diff>